<commit_message>
update prof excel file
</commit_message>
<xml_diff>
--- a/prof.xlsx
+++ b/prof.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Young Bakugo\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8AFA909-0667-4FE4-BA10-2881E31C12A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{891B1B53-A51F-4E82-8F1A-FA025ED527C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{FE02A65E-4A43-4665-9936-BB7035E63E9C}"/>
+    <workbookView xWindow="135" yWindow="0" windowWidth="20310" windowHeight="11520" xr2:uid="{FE02A65E-4A43-4665-9936-BB7035E63E9C}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,56 +25,29 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
-  <si>
-    <t>firstname</t>
-  </si>
-  <si>
-    <t>lastname</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>email</t>
   </si>
   <si>
-    <t>phone</t>
-  </si>
-  <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>/public/images/profs/FrancisLaurentFRPasseport35x45mmjpg_5e031965b7e3d.jpg</t>
-  </si>
-  <si>
     <t>Ratiarson</t>
   </si>
   <si>
     <t>Venot</t>
   </si>
   <si>
-    <t xml:space="preserve">pr_Titulaire </t>
-  </si>
-  <si>
     <t>rVenot@gmail.com</t>
   </si>
   <si>
     <t>louihaja@gmail.com</t>
   </si>
   <si>
-    <t>resp_Mention</t>
-  </si>
-  <si>
     <t>Louis Haja</t>
   </si>
   <si>
     <t>Rabetafika</t>
   </si>
   <si>
-    <t>/public/images/profs/istockphoto-516379821-612x612</t>
-  </si>
-  <si>
-    <t>/public/images/profs/photo-pour-l-identification-de-document-ou-passeport-homme-caucasien-mûr-dans-le-costume-126121929</t>
-  </si>
-  <si>
     <t>Andry</t>
   </si>
   <si>
@@ -87,12 +60,6 @@
     <t>andrybertin@gmail.com</t>
   </si>
   <si>
-    <t>profil_pic_path</t>
-  </si>
-  <si>
-    <t>/public/images/profs/istockphoto-1196211150-612x612</t>
-  </si>
-  <si>
     <t>Gezafy</t>
   </si>
   <si>
@@ -102,21 +69,6 @@
     <t>gilante@gmail.com</t>
   </si>
   <si>
-    <t>0341578963</t>
-  </si>
-  <si>
-    <t>0344548688</t>
-  </si>
-  <si>
-    <t>0334782152</t>
-  </si>
-  <si>
-    <t>0324782152</t>
-  </si>
-  <si>
-    <t>/public/images/profs/homme-portrait-sourire-300x300</t>
-  </si>
-  <si>
     <t>Randriamihaja</t>
   </si>
   <si>
@@ -126,22 +78,61 @@
     <t>josué@yahoo.fr</t>
   </si>
   <si>
-    <t>0321578965</t>
-  </si>
-  <si>
-    <t>/public/images/profs/istockphoto-1060680104-612x612</t>
-  </si>
-  <si>
     <t>Razafiarsoa</t>
   </si>
   <si>
-    <t>Stella</t>
-  </si>
-  <si>
-    <t>rStella@gmail.com</t>
-  </si>
-  <si>
-    <t>0347896152</t>
+    <t>photo_prof</t>
+  </si>
+  <si>
+    <t>nom</t>
+  </si>
+  <si>
+    <t>prenoms</t>
+  </si>
+  <si>
+    <t>titre</t>
+  </si>
+  <si>
+    <t>telephone</t>
+  </si>
+  <si>
+    <t>fonction</t>
+  </si>
+  <si>
+    <t>pr_Titulaire</t>
+  </si>
+  <si>
+    <t>rm</t>
+  </si>
+  <si>
+    <t>assistant_r</t>
+  </si>
+  <si>
+    <t>maitre_c</t>
+  </si>
+  <si>
+    <t>/public/images/istockphoto-1060680104-612x612</t>
+  </si>
+  <si>
+    <t>/public/images/homme-portrait-sourire-300x300</t>
+  </si>
+  <si>
+    <t>/public/images/photo-pour-l-identification-de-document-ou-passeport-homme-caucasien-mûr-dans-le-costume-126121929</t>
+  </si>
+  <si>
+    <t>/public/images/istockphoto-1196211150-612x612</t>
+  </si>
+  <si>
+    <t>/public/images/istockphoto-516379821-612x612</t>
+  </si>
+  <si>
+    <t>/public/images/FrancisLaurentFRPasseport35x45mmjpg_5e031965b7e3d.jpg</t>
+  </si>
+  <si>
+    <t>Pierrette</t>
+  </si>
+  <si>
+    <t>rPierrette@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -511,163 +502,179 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD601A06-790A-4242-AA9B-7E11E32A5297}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="2">
+        <v>261341578963</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
+      <c r="G3" s="2">
+        <v>2610344548688</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="2">
+        <v>261334782152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E5" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>25</v>
+      <c r="F5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="2">
+        <v>261324782152</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>33</v>
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="2">
+        <v>261321578965</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
         <v>34</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>38</v>
+      <c r="G7" s="2">
+        <v>261347896152</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{6A22A5F4-CCF6-4134-91F2-22AE1E47736E}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{644B12D3-E4B3-4639-9998-CD9A487FF623}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{DFF397BC-6E96-496A-95C7-3F1EC9319AD5}"/>
-    <hyperlink ref="E5" r:id="rId4" xr:uid="{0A2497C5-108E-40B4-97AA-B6C10586D62F}"/>
-    <hyperlink ref="E6" r:id="rId5" xr:uid="{95EA3E24-2709-4A69-8068-D13DA4BD3871}"/>
-    <hyperlink ref="E7" r:id="rId6" xr:uid="{0B35D134-49DB-49A3-A3F0-A6A6ADA48773}"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{6A22A5F4-CCF6-4134-91F2-22AE1E47736E}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{644B12D3-E4B3-4639-9998-CD9A487FF623}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{DFF397BC-6E96-496A-95C7-3F1EC9319AD5}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{0A2497C5-108E-40B4-97AA-B6C10586D62F}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{95EA3E24-2709-4A69-8068-D13DA4BD3871}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{0B35D134-49DB-49A3-A3F0-A6A6ADA48773}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>